<commit_message>
update tasks and add start date column
</commit_message>
<xml_diff>
--- a/ADMINISTRATIVE/Tasks_and_Schedules.xlsx
+++ b/ADMINISTRATIVE/Tasks_and_Schedules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawn3\Documents\Projects\MATERIAL_TRANSFER_ROBOT_2026\ADMINISTRATIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64701FD-B2F3-4A3F-AF25-EBD5F0ED0E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340FDDF-6A46-4B51-B572-C01A83DFA783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C5FB643-9C8C-4A32-B14C-09FCE1F64F30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Lalithesh</t>
   </si>
   <si>
-    <t>Map Switching Logic using Travelled Distance via ZED Mini</t>
-  </si>
-  <si>
     <t>Integration of Aruco Based Localization to Map Switching Logic</t>
   </si>
   <si>
@@ -81,6 +78,15 @@
   </si>
   <si>
     <t>Measure Standoff Distance &amp; Angular Resolution for Aruco Markers</t>
+  </si>
+  <si>
+    <t>Map Switching Logic using Travelled Distance</t>
+  </si>
+  <si>
+    <t>Date of Start</t>
+  </si>
+  <si>
+    <t>Setup Jetson</t>
   </si>
 </sst>
 </file>
@@ -498,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAC5248-6238-4344-9CEB-611CC72BEF89}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,10 +515,11 @@
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,38 +530,47 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3">
-        <v>46000</v>
+        <v>45999</v>
       </c>
       <c r="D2" s="3">
-        <v>46007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46010</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3">
-        <v>46006</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>46000</v>
+      </c>
+      <c r="E3" s="3">
+        <v>46007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -562,63 +578,74 @@
       <c r="C4" s="3">
         <v>46006</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>46006</v>
+      </c>
+      <c r="D5" s="3">
+        <v>46007</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5">
-        <v>46000</v>
-      </c>
-      <c r="D5" s="5">
-        <v>46003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5">
+        <v>46000</v>
+      </c>
+      <c r="D6" s="5">
+        <v>46000</v>
+      </c>
+      <c r="E6" s="5">
+        <v>46003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>46006</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7">
-        <v>46000</v>
-      </c>
-      <c r="D7" s="7">
-        <v>46003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="7">
-        <v>46006</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46000</v>
+      </c>
+      <c r="D8" s="7">
+        <v>46000</v>
+      </c>
+      <c r="E8" s="7">
+        <v>46003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>10</v>
@@ -626,7 +653,21 @@
       <c r="C9" s="7">
         <v>46006</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7">
+        <v>46006</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>